<commit_message>
copy paste from observable example
</commit_message>
<xml_diff>
--- a/data/nodes_links.xlsx
+++ b/data/nodes_links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qichun/Documents/GitHub/learningD3_day2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5304B612-32EF-FC4B-A199-69A6D32DC1D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60273E73-A9D5-8643-80F1-CA0BEF2FE52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15880" yWindow="-24020" windowWidth="28800" windowHeight="18060" activeTab="1" xr2:uid="{934D0E16-5AB4-FD45-9464-E4CAA10E6571}"/>
+    <workbookView xWindow="-10880" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{934D0E16-5AB4-FD45-9464-E4CAA10E6571}"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes" sheetId="1" r:id="rId1"/>
@@ -639,7 +639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624398E6-BC4D-A34A-9EAC-5BA2239C655B}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H38"/>
     </sheetView>
   </sheetViews>
@@ -686,8 +686,8 @@
         <v>1</v>
       </c>
       <c r="H2" t="str">
-        <f>"{"&amp;CHAR(34)&amp;"id"&amp;CHAR(34)&amp;": "&amp;A2&amp;", "&amp;CHAR(34)&amp;"first_name"&amp;CHAR(34)&amp;":  "&amp;CHAR(34)&amp;B2&amp;CHAR(34)&amp;", "&amp;CHAR(34)&amp;"team"&amp;CHAR(34)&amp;":  "&amp;CHAR(34)&amp;D2&amp;CHAR(34)&amp;", "&amp;CHAR(34)&amp;"group"&amp;CHAR(34)&amp;":  "&amp;E2&amp;"},"</f>
-        <v>{"id": 1, "first_name":  "Albus", "team":  "Head Master", "group":  1},</v>
+        <f>"{"&amp;CHAR(34)&amp;"id"&amp;CHAR(34)&amp;": "&amp;A2&amp;", "&amp;CHAR(34)&amp;"first_name"&amp;CHAR(34)&amp;":  "&amp;CHAR(34)&amp;B2&amp;CHAR(34)&amp;", "&amp;CHAR(34)&amp;"last_name"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;C2&amp;CHAR(34)&amp;", "&amp;CHAR(34)&amp;"team"&amp;CHAR(34)&amp;":  "&amp;CHAR(34)&amp;D2&amp;CHAR(34)&amp;", "&amp;CHAR(34)&amp;"group"&amp;CHAR(34)&amp;":  "&amp;E2&amp;"},"</f>
+        <v>{"id": 1, "first_name":  "Albus", "last_name": "Dumbledore", "team":  "Head Master", "group":  1},</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -707,8 +707,8 @@
         <v>2</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H38" si="0">"{"&amp;CHAR(34)&amp;"id"&amp;CHAR(34)&amp;": "&amp;A3&amp;", "&amp;CHAR(34)&amp;"first_name"&amp;CHAR(34)&amp;":  "&amp;CHAR(34)&amp;B3&amp;CHAR(34)&amp;", "&amp;CHAR(34)&amp;"team"&amp;CHAR(34)&amp;":  "&amp;CHAR(34)&amp;D3&amp;CHAR(34)&amp;", "&amp;CHAR(34)&amp;"group"&amp;CHAR(34)&amp;":  "&amp;E3&amp;"},"</f>
-        <v>{"id": 2, "first_name":  "Minerva", "team":  "Gryffindor", "group":  2},</v>
+        <f t="shared" ref="H3:H38" si="0">"{"&amp;CHAR(34)&amp;"id"&amp;CHAR(34)&amp;": "&amp;A3&amp;", "&amp;CHAR(34)&amp;"first_name"&amp;CHAR(34)&amp;":  "&amp;CHAR(34)&amp;B3&amp;CHAR(34)&amp;", "&amp;CHAR(34)&amp;"last_name"&amp;CHAR(34)&amp;": "&amp;CHAR(34)&amp;C3&amp;CHAR(34)&amp;", "&amp;CHAR(34)&amp;"team"&amp;CHAR(34)&amp;":  "&amp;CHAR(34)&amp;D3&amp;CHAR(34)&amp;", "&amp;CHAR(34)&amp;"group"&amp;CHAR(34)&amp;":  "&amp;E3&amp;"},"</f>
+        <v>{"id": 2, "first_name":  "Minerva", "last_name": "McGonagall", "team":  "Gryffindor", "group":  2},</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -729,7 +729,7 @@
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 3, "first_name":  "Pomona", "team":  "Hufflepuff", "group":  2},</v>
+        <v>{"id": 3, "first_name":  "Pomona", "last_name": "Sprout", "team":  "Hufflepuff", "group":  2},</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -750,7 +750,7 @@
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 4, "first_name":  "Filius", "team":  "Ravenclaw", "group":  2},</v>
+        <v>{"id": 4, "first_name":  "Filius", "last_name": "Flitwick", "team":  "Ravenclaw", "group":  2},</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -771,7 +771,7 @@
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 5, "first_name":  "Severus", "team":  "Slytherin", "group":  2},</v>
+        <v>{"id": 5, "first_name":  "Severus", "last_name": "Snape", "team":  "Slytherin", "group":  2},</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -792,7 +792,7 @@
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 6, "first_name":  "Harry", "team":  "Gryffindor", "group":  3},</v>
+        <v>{"id": 6, "first_name":  "Harry", "last_name": "Potter", "team":  "Gryffindor", "group":  3},</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -813,7 +813,7 @@
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 7, "first_name":  "Hermione", "team":  "Gryffindor", "group":  3},</v>
+        <v>{"id": 7, "first_name":  "Hermione", "last_name": "Granger", "team":  "Gryffindor", "group":  3},</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -834,7 +834,7 @@
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 8, "first_name":  "Ron", "team":  "Gryffindor", "group":  3},</v>
+        <v>{"id": 8, "first_name":  "Ron", "last_name": "Weasley", "team":  "Gryffindor", "group":  3},</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -855,7 +855,7 @@
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 9, "first_name":  "Neville", "team":  "Gryffindor", "group":  3},</v>
+        <v>{"id": 9, "first_name":  "Neville", "last_name": "Longbottom", "team":  "Gryffindor", "group":  3},</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -876,7 +876,7 @@
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 10, "first_name":  "Ginny", "team":  "Gryffindor", "group":  3},</v>
+        <v>{"id": 10, "first_name":  "Ginny", "last_name": "Weasley", "team":  "Gryffindor", "group":  3},</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -897,7 +897,7 @@
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 11, "first_name":  "Seamus", "team":  "Gryffindor", "group":  3},</v>
+        <v>{"id": 11, "first_name":  "Seamus", "last_name": "Finnigan", "team":  "Gryffindor", "group":  3},</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -918,7 +918,7 @@
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 12, "first_name":  "Dean", "team":  "Gryffindor", "group":  3},</v>
+        <v>{"id": 12, "first_name":  "Dean", "last_name": "Thomas", "team":  "Gryffindor", "group":  3},</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -939,7 +939,7 @@
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 13, "first_name":  "Parvati", "team":  "Gryffindor", "group":  3},</v>
+        <v>{"id": 13, "first_name":  "Parvati", "last_name": "Patil", "team":  "Gryffindor", "group":  3},</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -960,7 +960,7 @@
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 14, "first_name":  "Lavender", "team":  "Gryffindor", "group":  3},</v>
+        <v>{"id": 14, "first_name":  "Lavender", "last_name": "Brown", "team":  "Gryffindor", "group":  3},</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -981,7 +981,7 @@
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 15, "first_name":  "Colin", "team":  "Gryffindor", "group":  3},</v>
+        <v>{"id": 15, "first_name":  "Colin", "last_name": "Creevey", "team":  "Gryffindor", "group":  3},</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1002,7 +1002,7 @@
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 16, "first_name":  "Fred", "team":  "Gryffindor", "group":  3},</v>
+        <v>{"id": 16, "first_name":  "Fred", "last_name": "Weasley", "team":  "Gryffindor", "group":  3},</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 17, "first_name":  "George", "team":  "Gryffindor", "group":  3},</v>
+        <v>{"id": 17, "first_name":  "George", "last_name": "Weasley", "team":  "Gryffindor", "group":  3},</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 18, "first_name":  "Cedric", "team":  "Hufflepuff", "group":  3},</v>
+        <v>{"id": 18, "first_name":  "Cedric", "last_name": "Diggory", "team":  "Hufflepuff", "group":  3},</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1065,7 +1065,7 @@
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 19, "first_name":  "Hannah", "team":  "Hufflepuff", "group":  3},</v>
+        <v>{"id": 19, "first_name":  "Hannah", "last_name": "Abbott", "team":  "Hufflepuff", "group":  3},</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 20, "first_name":  "Ernie", "team":  "Hufflepuff", "group":  3},</v>
+        <v>{"id": 20, "first_name":  "Ernie", "last_name": "Macmillan", "team":  "Hufflepuff", "group":  3},</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1107,7 +1107,7 @@
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 21, "first_name":  "Justin", "team":  "Hufflepuff", "group":  3},</v>
+        <v>{"id": 21, "first_name":  "Justin", "last_name": "Finch-Fletchley", "team":  "Hufflepuff", "group":  3},</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1128,7 +1128,7 @@
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 22, "first_name":  "Susan", "team":  "Hufflepuff", "group":  3},</v>
+        <v>{"id": 22, "first_name":  "Susan", "last_name": "Bones", "team":  "Hufflepuff", "group":  3},</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 23, "first_name":  "Luna", "team":  "Ravenclaw", "group":  3},</v>
+        <v>{"id": 23, "first_name":  "Luna", "last_name": "Lovegood", "team":  "Ravenclaw", "group":  3},</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 24, "first_name":  "Cho", "team":  "Ravenclaw", "group":  3},</v>
+        <v>{"id": 24, "first_name":  "Cho", "last_name": "Chang", "team":  "Ravenclaw", "group":  3},</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 25, "first_name":  "Padma", "team":  "Ravenclaw", "group":  3},</v>
+        <v>{"id": 25, "first_name":  "Padma", "last_name": "Patil", "team":  "Ravenclaw", "group":  3},</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1212,7 +1212,7 @@
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 26, "first_name":  "Marietta", "team":  "Ravenclaw", "group":  3},</v>
+        <v>{"id": 26, "first_name":  "Marietta", "last_name": "Edgecombe", "team":  "Ravenclaw", "group":  3},</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1233,7 +1233,7 @@
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 27, "first_name":  "Michael", "team":  "Ravenclaw", "group":  3},</v>
+        <v>{"id": 27, "first_name":  "Michael", "last_name": "Corner", "team":  "Ravenclaw", "group":  3},</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1254,7 +1254,7 @@
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 28, "first_name":  "Terry", "team":  "Ravenclaw", "group":  3},</v>
+        <v>{"id": 28, "first_name":  "Terry", "last_name": "Boot", "team":  "Ravenclaw", "group":  3},</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1275,7 +1275,7 @@
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 29, "first_name":  "Anthony", "team":  "Ravenclaw", "group":  3},</v>
+        <v>{"id": 29, "first_name":  "Anthony", "last_name": "Goldstein", "team":  "Ravenclaw", "group":  3},</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1296,7 +1296,7 @@
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 30, "first_name":  "Draco", "team":  "Slytherin", "group":  3},</v>
+        <v>{"id": 30, "first_name":  "Draco", "last_name": "Malfoy", "team":  "Slytherin", "group":  3},</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1317,7 +1317,7 @@
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 31, "first_name":  "Pansy", "team":  "Slytherin", "group":  3},</v>
+        <v>{"id": 31, "first_name":  "Pansy", "last_name": "Parkinson", "team":  "Slytherin", "group":  3},</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 32, "first_name":  "Gregory", "team":  "Slytherin", "group":  3},</v>
+        <v>{"id": 32, "first_name":  "Gregory", "last_name": "Goyle", "team":  "Slytherin", "group":  3},</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1359,7 +1359,7 @@
       </c>
       <c r="H34" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 33, "first_name":  "Vicent", "team":  "Slytherin", "group":  3},</v>
+        <v>{"id": 33, "first_name":  "Vicent", "last_name": "Crabbe", "team":  "Slytherin", "group":  3},</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1380,7 +1380,7 @@
       </c>
       <c r="H35" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 34, "first_name":  "Millicent", "team":  "Slytherin", "group":  3},</v>
+        <v>{"id": 34, "first_name":  "Millicent", "last_name": "Bulstrode", "team":  "Slytherin", "group":  3},</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="H36" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 35, "first_name":  "Blaise", "team":  "Slytherin", "group":  3},</v>
+        <v>{"id": 35, "first_name":  "Blaise", "last_name": "Zabini", "team":  "Slytherin", "group":  3},</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1422,7 +1422,7 @@
       </c>
       <c r="H37" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 36, "first_name":  "Daphne", "team":  "Slytherin", "group":  3},</v>
+        <v>{"id": 36, "first_name":  "Daphne", "last_name": "Greengrass", "team":  "Slytherin", "group":  3},</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1443,7 +1443,7 @@
       </c>
       <c r="H38" t="str">
         <f t="shared" si="0"/>
-        <v>{"id": 37, "first_name":  "Theodore", "team":  "Slytherin", "group":  3},</v>
+        <v>{"id": 37, "first_name":  "Theodore", "last_name": "Nott", "team":  "Slytherin", "group":  3},</v>
       </c>
     </row>
   </sheetData>
@@ -1456,7 +1456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17684B4F-5C20-8745-9EB4-E29BA7B6660E}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>

</xml_diff>